<commit_message>
update manifests, date: 2021-02-06, last lines (exp, sim, neg): (16, 12, 5)
</commit_message>
<xml_diff>
--- a/manifests/Negative_Manifest.xlsx
+++ b/manifests/Negative_Manifest.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8250" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -52,6 +52,74 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -322,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -331,7 +399,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
     <col width="10.1796875" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="10.08984375" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="22.36328125" bestFit="1" customWidth="1" min="2" max="2"/>
     <col width="15.1796875" bestFit="1" customWidth="1" min="3" max="3"/>
     <col width="14" bestFit="1" customWidth="1" min="4" max="4"/>
     <col width="12.36328125" bestFit="1" customWidth="1" min="5" max="5"/>
@@ -364,7 +432,87 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>n1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>n1_IMG_3178.jpeg</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>n2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>n2_IMG_3180.jpeg</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>n3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>n3_IMG_3174.jpeg</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update manifests, date: 2021-02-07, IDs (exp, sim, neg): (14, 10, 3)
</commit_message>
<xml_diff>
--- a/manifests/Negative_Manifest.xlsx
+++ b/manifests/Negative_Manifest.xlsx
@@ -1,33 +1,57 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dkess\OneDrive\Documents\CWRU\Macro\Python\Macro-Citizen-Science\manifests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8250" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8250"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>!subject_ID</t>
+  </si>
+  <si>
+    <t>#file_name</t>
+  </si>
+  <si>
+    <t>#training_subject</t>
+  </si>
+  <si>
+    <t>#feedback_1_id</t>
+  </si>
+  <si>
+    <t>#classification</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,80 +70,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -385,132 +350,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col width="10.1796875" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="22.36328125" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="15.1796875" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="14" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="12.36328125" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>!subject_ID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>#file_name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>#training_subject</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>#feedback_1_id</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>#classification</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>n1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>n1_IMG_3178.jpeg</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>no_meltpatch</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>negative</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>n2</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>n2_IMG_3180.jpeg</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>no_meltpatch</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>negative</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>n3</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>n3_IMG_3174.jpeg</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>no_meltpatch</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>negative</t>
-        </is>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update manifests, date: 2021-02-11, last lines (exp, sim, neg): (30, 70, 26)
</commit_message>
<xml_diff>
--- a/manifests/Negative_Manifest.xlsx
+++ b/manifests/Negative_Manifest.xlsx
@@ -390,10 +390,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E25"/>
+    <sheetView tabSelected="1" zoomScale="66" workbookViewId="0">
+      <selection activeCell="E29" sqref="A2:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -548,7 +548,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>n5_IMG_3175.jpeg</t>
+          <t>n5_IMG_3176.jpeg</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -575,7 +575,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>n6_IMG_3175HorFlip.jpeg</t>
+          <t>n6_IMG_3176HorFlip.jpeg</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -602,7 +602,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>n7_IMG_3175HorVertFlip.jpeg</t>
+          <t>n7_IMG_3176HorVertFlip.jpeg</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>n8_IMG_3175VertFlip.jpeg</t>
+          <t>n8_IMG_3176VertFlip.jpeg</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -656,7 +656,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>n9_IMG_3176.jpeg</t>
+          <t>n9_IMG_3177.jpeg</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -683,7 +683,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>n10_IMG_3176HorFlip.jpeg</t>
+          <t>n10_IMG_3177HorFlip.jpeg</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -710,7 +710,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>n11_IMG_3176HorVertFlip.jpeg</t>
+          <t>n11_IMG_3177HorVertFlip.jpeg</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -737,7 +737,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>n12_IMG_3176VertFlip.jpeg</t>
+          <t>n12_IMG_3177VertFlip.jpeg</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -764,7 +764,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>n13_IMG_3177.jpeg</t>
+          <t>n13_IMG_3178.jpeg</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -791,7 +791,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>n14_IMG_3177HorFlip.jpeg</t>
+          <t>n14_IMG_3178HorFlip.jpeg</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -818,7 +818,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>n15_IMG_3177HorVertFlip.jpeg</t>
+          <t>n15_IMG_3178HorVertFlip.jpeg</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -845,7 +845,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>n16_IMG_3177VertFlip.jpeg</t>
+          <t>n16_IMG_3178VertFlip.jpeg</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -872,7 +872,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>n17_IMG_3178.jpeg</t>
+          <t>n17_IMG_3179.jpeg</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -899,7 +899,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>n18_IMG_3178HorFlip.jpeg</t>
+          <t>n18_IMG_3179HorFlip.jpeg</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -926,7 +926,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>n19_IMG_3178HorVertFlip.jpeg</t>
+          <t>n19_IMG_3179HorVertFlip.jpeg</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>n20_IMG_3178VertFlip.jpeg</t>
+          <t>n20_IMG_3179VertFlip.jpeg</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -980,7 +980,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>n21_IMG_3179.jpeg</t>
+          <t>n21_IMG_3180.jpeg</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1007,7 +1007,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>n22_IMG_3179HorFlip.jpeg</t>
+          <t>n22_IMG_3180HorFlip.jpeg</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1034,7 +1034,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>n23_IMG_3179HorVertFlip.jpeg</t>
+          <t>n23_IMG_3180HorVertFlip.jpeg</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1061,7 +1061,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>n24_IMG_3179VertFlip.jpeg</t>
+          <t>n24_IMG_3180VertFlip.jpeg</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1075,114 +1075,6 @@
         </is>
       </c>
       <c r="E25" t="inlineStr">
-        <is>
-          <t>negative</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>n25</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>n25_IMG_3180.jpeg</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>no_meltpatch</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>negative</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>n26</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>n26_IMG_3180HorFlip.jpeg</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>no_meltpatch</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>negative</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>n27</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>n27_IMG_3180HorVertFlip.jpeg</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>no_meltpatch</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>negative</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>n28</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>n28_IMG_3180VertFlip.jpeg</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>no_meltpatch</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
         <is>
           <t>negative</t>
         </is>

</xml_diff>

<commit_message>
update manifests, date: 2021-02-12, last lines (exp, sim, neg): (98, 138, 40)
</commit_message>
<xml_diff>
--- a/manifests/Negative_Manifest.xlsx
+++ b/manifests/Negative_Manifest.xlsx
@@ -390,10 +390,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" workbookViewId="0">
-      <selection activeCell="E29" sqref="A2:E29"/>
+      <selection activeCell="A26" sqref="A26:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -1080,7 +1080,385 @@
         </is>
       </c>
     </row>
-    <row r="26"/>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>n25</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>n25_IMG_3070 - Copy.jpeg</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>n26</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>n26_IMG_3070.jpeg</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>n27</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>n27_IMG_3070HorFlip - Copy.jpeg</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>n28</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>n28_IMG_3070HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>n29</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>n29_IMG_3070HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>n30</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>n30_IMG_3070VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>n31</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>n31_IMG_3072.jpeg</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>n32</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>n32_IMG_3072HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>n33</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>n33_IMG_3072HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>n34</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>n34_IMG_3072VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>n35</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>n35_IMG_3073.jpeg</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>n36</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>n36_IMG_3073HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>n37</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>n37_IMG_3073HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>n38</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>n38_IMG_3073VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="40"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update manifests, date: 2021-02-13, last lines (exp, sim, neg): (154, 170, 76)
</commit_message>
<xml_diff>
--- a/manifests/Negative_Manifest.xlsx
+++ b/manifests/Negative_Manifest.xlsx
@@ -390,10 +390,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" zoomScale="66" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:E52"/>
+      <selection activeCell="A40" sqref="A40:E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>n52_IMG_3070.jpeg</t>
+          <t>n52_IMG_3178HorFlip.jpeg</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1844,7 +1844,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>n53_IMG_3070HorFlip.jpeg</t>
+          <t>n53_IMG_3178HorVertFlip.jpeg</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1871,7 +1871,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>n54_IMG_3070HorVertFlip.jpeg</t>
+          <t>n54_IMG_3178VertFlip.jpeg</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1898,7 +1898,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>n55_IMG_3070VertFlip.jpeg</t>
+          <t>n55_IMG_3179.jpeg</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1925,7 +1925,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>n56_IMG_3072.jpeg</t>
+          <t>n56_IMG_3179HorFlip.jpeg</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1952,7 +1952,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>n57_IMG_3072HorFlip.jpeg</t>
+          <t>n57_IMG_3179HorVertFlip.jpeg</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1979,7 +1979,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>n58_IMG_3072HorVertFlip.jpeg</t>
+          <t>n58_IMG_3179VertFlip.jpeg</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2006,7 +2006,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>n59_IMG_3072VertFlip.jpeg</t>
+          <t>n59_IMG_3180.jpeg</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2033,7 +2033,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>n60_IMG_3073.jpeg</t>
+          <t>n60_IMG_3180HorFlip.jpeg</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2060,7 +2060,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>n61_IMG_3073HorFlip.jpeg</t>
+          <t>n61_IMG_3180HorVertFlip.jpeg</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2087,7 +2087,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>n62_IMG_3073HorVertFlip.jpeg</t>
+          <t>n62_IMG_3180VertFlip.jpeg</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2114,7 +2114,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>n63_IMG_3073VertFlip.jpeg</t>
+          <t>n63_IMG_3070.jpeg</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2128,6 +2128,303 @@
         </is>
       </c>
       <c r="E64" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>n64</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>n64_IMG_3070HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>n65</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>n65_IMG_3070HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>n66</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>n66_IMG_3070VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>n67</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>n67_IMG_3072.jpeg</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>n68</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>n68_IMG_3072HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>n69</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>n69_IMG_3072HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>n70</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>n70_IMG_3072VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>n71</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>n71_IMG_3073.jpeg</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>n72</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>n72_IMG_3073HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>n73</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>n73_IMG_3073HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>n74</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>n74_IMG_3073VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
         <is>
           <t>negative</t>
         </is>

</xml_diff>

<commit_message>
update manifests, date: 2021-02-13, last lines (exp, sim, neg): (154, 170, 100)
</commit_message>
<xml_diff>
--- a/manifests/Negative_Manifest.xlsx
+++ b/manifests/Negative_Manifest.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" zoomScale="66" workbookViewId="0">
       <selection activeCell="A40" sqref="A40:E75"/>
@@ -2754,6 +2754,330 @@
         </is>
       </c>
     </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>n87</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>n87_IMG_3088.jpeg</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>n88</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>n88_IMG_3088HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>n89</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>n89_IMG_3088HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>n90</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>n90_IMG_3088VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>n91</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>n91_IMG_3089.jpeg</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>n92</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>n92_IMG_3089HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>n93</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>n93_IMG_3089HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>n94</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>n94_IMG_3089VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>n95</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>n95_IMG_3091.jpeg</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>n96</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>n96_IMG_3091HorFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>n97</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>n97_IMG_3091HorVertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>n98</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>n98_IMG_3091VertFlip.jpeg</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>no_meltpatch</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>